<commit_message>
added selected particles with actual size weeks 1-2
</commit_message>
<xml_diff>
--- a/selected_particles/3_particle_selection.xlsx
+++ b/selected_particles/3_particle_selection.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="3_particle_selection" sheetId="1" r:id="rId3"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'3_particle_selection'!$A$1:$H$31</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>frame</t>
   </si>
@@ -26,6 +28,9 @@
   </si>
   <si>
     <t>size</t>
+  </si>
+  <si>
+    <t>actual_size</t>
   </si>
   <si>
     <t>video</t>
@@ -91,7 +96,7 @@
   <cols>
     <col customWidth="1" min="3" max="3" width="8.29"/>
     <col customWidth="1" min="4" max="4" width="3.43"/>
-    <col customWidth="1" min="5" max="5" width="4.0"/>
+    <col customWidth="1" min="5" max="5" width="12.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -116,8 +121,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" hidden="1">
       <c r="A2" s="1">
         <v>0.0</v>
       </c>
@@ -133,10 +141,11 @@
       <c r="E2" s="1">
         <v>14.0379062351168</v>
       </c>
-      <c r="F2" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H2" s="1">
         <v>0.0</v>
       </c>
     </row>
@@ -157,9 +166,12 @@
         <v>10.3936741766184</v>
       </c>
       <c r="F3" s="1">
-        <v>3.0</v>
+        <v>16.0</v>
       </c>
       <c r="G3" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H3" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -180,9 +192,12 @@
         <v>14.0687187633112</v>
       </c>
       <c r="F4" s="1">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="G4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H4" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -203,13 +218,16 @@
         <v>18.1119457240088</v>
       </c>
       <c r="F5" s="1">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
       <c r="G5" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>3.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6" hidden="1">
       <c r="A6" s="1">
         <v>0.0</v>
       </c>
@@ -225,14 +243,15 @@
       <c r="E6" s="1">
         <v>11.5202037578683</v>
       </c>
-      <c r="F6" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>3.0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" hidden="1">
       <c r="A7" s="1">
         <v>0.0</v>
       </c>
@@ -248,14 +267,15 @@
       <c r="E7" s="1">
         <v>22.6110324984367</v>
       </c>
-      <c r="F7" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>3.0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" hidden="1">
       <c r="A8" s="1">
         <v>0.0</v>
       </c>
@@ -271,14 +291,15 @@
       <c r="E8" s="1">
         <v>11.7036713770856</v>
       </c>
-      <c r="F8" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>3.0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" hidden="1">
       <c r="A9" s="1">
         <v>0.0</v>
       </c>
@@ -294,14 +315,15 @@
       <c r="E9" s="1">
         <v>10.6116886011029</v>
       </c>
-      <c r="F9" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>3.0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10" hidden="1">
       <c r="A10" s="1">
         <v>0.0</v>
       </c>
@@ -317,14 +339,15 @@
       <c r="E10" s="1">
         <v>14.5856034102064</v>
       </c>
-      <c r="F10" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>3.0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11" hidden="1">
       <c r="A11" s="1">
         <v>0.0</v>
       </c>
@@ -340,10 +363,11 @@
       <c r="E11" s="1">
         <v>13.2032873593792</v>
       </c>
-      <c r="F11" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.0</v>
       </c>
     </row>
@@ -364,9 +388,12 @@
         <v>14.7038090068724</v>
       </c>
       <c r="F12" s="1">
-        <v>3.0</v>
+        <v>7.5</v>
       </c>
       <c r="G12" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H12" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -387,13 +414,16 @@
         <v>22.4437086137302</v>
       </c>
       <c r="F13" s="1">
-        <v>3.0</v>
+        <v>5.5</v>
       </c>
       <c r="G13" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>3.0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14" hidden="1">
       <c r="A14" s="1">
         <v>0.0</v>
       </c>
@@ -409,14 +439,15 @@
       <c r="E14" s="1">
         <v>13.6294612000739</v>
       </c>
-      <c r="F14" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>3.0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" hidden="1">
       <c r="A15" s="1">
         <v>0.0</v>
       </c>
@@ -432,14 +463,15 @@
       <c r="E15" s="1">
         <v>20.0448091063999</v>
       </c>
-      <c r="F15" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>3.0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" hidden="1">
       <c r="A16" s="1">
         <v>0.0</v>
       </c>
@@ -455,14 +487,15 @@
       <c r="E16" s="1">
         <v>11.9370765231009</v>
       </c>
-      <c r="F16" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>3.0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17" hidden="1">
       <c r="A17" s="1">
         <v>0.0</v>
       </c>
@@ -478,14 +511,15 @@
       <c r="E17" s="1">
         <v>20.7779729058842</v>
       </c>
-      <c r="F17" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>3.0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18" hidden="1">
       <c r="A18" s="1">
         <v>0.0</v>
       </c>
@@ -501,14 +535,15 @@
       <c r="E18" s="1">
         <v>14.7528638951441</v>
       </c>
-      <c r="F18" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>3.0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19" hidden="1">
       <c r="A19" s="1">
         <v>0.0</v>
       </c>
@@ -524,10 +559,11 @@
       <c r="E19" s="1">
         <v>19.4902310355539</v>
       </c>
-      <c r="F19" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H19" s="1">
         <v>0.0</v>
       </c>
     </row>
@@ -548,13 +584,16 @@
         <v>16.9237110511266</v>
       </c>
       <c r="F20" s="1">
-        <v>3.0</v>
+        <v>21.0</v>
       </c>
       <c r="G20" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>3.0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21" hidden="1">
       <c r="A21" s="1">
         <v>0.0</v>
       </c>
@@ -570,14 +609,15 @@
       <c r="E21" s="1">
         <v>14.2183845377893</v>
       </c>
-      <c r="F21" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>3.0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22" hidden="1">
       <c r="A22" s="1">
         <v>0.0</v>
       </c>
@@ -593,14 +633,15 @@
       <c r="E22" s="1">
         <v>12.7599848134408</v>
       </c>
-      <c r="F22" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>3.0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23" hidden="1">
       <c r="A23" s="1">
         <v>0.0</v>
       </c>
@@ -616,10 +657,11 @@
       <c r="E23" s="1">
         <v>19.6983091117416</v>
       </c>
-      <c r="F23" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H23" s="1">
         <v>0.0</v>
       </c>
     </row>
@@ -640,9 +682,12 @@
         <v>9.88316110754941</v>
       </c>
       <c r="F24" s="1">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="G24" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H24" s="1">
         <v>1.0</v>
       </c>
     </row>
@@ -662,14 +707,15 @@
       <c r="E25" s="1">
         <v>12.9196591576905</v>
       </c>
-      <c r="F25" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>3.0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26" hidden="1">
       <c r="A26" s="1">
         <v>0.0</v>
       </c>
@@ -685,10 +731,11 @@
       <c r="E26" s="1">
         <v>14.1526049606967</v>
       </c>
-      <c r="F26" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F26" s="1"/>
       <c r="G26" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="H26" s="1">
         <v>0.0</v>
       </c>
     </row>
@@ -709,13 +756,16 @@
         <v>13.4586877379046</v>
       </c>
       <c r="F27" s="1">
-        <v>3.0</v>
+        <v>10.0</v>
       </c>
       <c r="G27" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>3.0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="28" hidden="1">
       <c r="A28" s="1">
         <v>0.0</v>
       </c>
@@ -731,14 +781,15 @@
       <c r="E28" s="1">
         <v>14.5910833293996</v>
       </c>
-      <c r="F28" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F28" s="1"/>
       <c r="G28" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>3.0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" hidden="1">
       <c r="A29" s="1">
         <v>0.0</v>
       </c>
@@ -754,14 +805,15 @@
       <c r="E29" s="1">
         <v>11.4334819364288</v>
       </c>
-      <c r="F29" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>3.0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30" hidden="1">
       <c r="A30" s="1">
         <v>0.0</v>
       </c>
@@ -777,14 +829,15 @@
       <c r="E30" s="1">
         <v>13.5066639987707</v>
       </c>
-      <c r="F30" s="1">
-        <v>3.0</v>
-      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>3.0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31" hidden="1">
       <c r="A31" s="1">
         <v>0.0</v>
       </c>
@@ -801,13 +854,23 @@
         <v>10.7616143744154</v>
       </c>
       <c r="F31" s="1">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="G31" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="$A$1:$H$31">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>